<commit_message>
added runway condition RWC
</commit_message>
<xml_diff>
--- a/data-raw/metar_config.xlsx
+++ b/data-raw/metar_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mat\Documents\R\metar\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE1D0DF-943C-47DD-96D8-2255EFE85C51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BE9786-FD14-4914-B5E1-C0D07DFCC374}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" tabRatio="731" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1575" uniqueCount="1168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1580" uniqueCount="1170">
   <si>
     <t>FG</t>
   </si>
@@ -3547,6 +3547,12 @@
   </si>
   <si>
     <t>Empty groups</t>
+  </si>
+  <si>
+    <t>rwc</t>
+  </si>
+  <si>
+    <t>Runway Condition</t>
   </si>
 </sst>
 </file>
@@ -3880,10 +3886,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2900C6E8-A8B5-4407-A7A1-C33011B0ABA6}">
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:C42"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4516,6 +4522,9 @@
       <c r="C30" t="s">
         <v>1049</v>
       </c>
+      <c r="E30" s="10" t="s">
+        <v>145</v>
+      </c>
       <c r="F30" t="s">
         <v>122</v>
       </c>
@@ -4594,13 +4603,13 @@
     </row>
     <row r="34" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>125</v>
+        <v>1168</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>1111</v>
+        <v>1168</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>1105</v>
+        <v>1169</v>
       </c>
       <c r="F34" s="10" t="s">
         <v>122</v>
@@ -4611,13 +4620,13 @@
     </row>
     <row r="35" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>1102</v>
+        <v>125</v>
       </c>
       <c r="B35" s="10" t="s">
         <v>1111</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="F35" s="10" t="s">
         <v>122</v>
@@ -4628,7 +4637,7 @@
     </row>
     <row r="36" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B36" s="10" t="s">
         <v>1111</v>
@@ -4645,39 +4654,30 @@
     </row>
     <row r="37" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>1096</v>
+        <v>1103</v>
       </c>
       <c r="B37" s="10" t="s">
         <v>1111</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>1094</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>183</v>
+        <v>1104</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>1056</v>
+        <v>122</v>
       </c>
       <c r="G37" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="H37" s="10">
-        <v>-180</v>
-      </c>
-      <c r="I37" s="10">
-        <v>180</v>
-      </c>
     </row>
     <row r="38" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="B38" s="10" t="s">
         <v>1111</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>183</v>
@@ -4689,24 +4689,24 @@
         <v>0</v>
       </c>
       <c r="H38" s="10">
-        <v>-90</v>
+        <v>-180</v>
       </c>
       <c r="I38" s="10">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="B39" s="10" t="s">
         <v>1111</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>1099</v>
+        <v>1095</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F39" s="10" t="s">
         <v>1056</v>
@@ -4715,38 +4715,47 @@
         <v>0</v>
       </c>
       <c r="H39" s="10">
-        <v>-999</v>
+        <v>-90</v>
       </c>
       <c r="I39" s="10">
-        <v>9999</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>1100</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>1098</v>
       </c>
       <c r="B40" s="10" t="s">
         <v>1111</v>
       </c>
-      <c r="C40" t="s">
-        <v>1101</v>
-      </c>
-      <c r="F40" t="s">
-        <v>122</v>
-      </c>
-      <c r="G40" t="b">
+      <c r="C40" s="10" t="s">
+        <v>1099</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G40" s="10" t="b">
         <v>0</v>
+      </c>
+      <c r="H40" s="10">
+        <v>-999</v>
+      </c>
+      <c r="I40" s="10">
+        <v>9999</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1106</v>
+        <v>1100</v>
       </c>
       <c r="B41" s="10" t="s">
         <v>1111</v>
       </c>
       <c r="C41" t="s">
-        <v>1112</v>
+        <v>1101</v>
       </c>
       <c r="F41" t="s">
         <v>122</v>
@@ -4757,13 +4766,13 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>1113</v>
+        <v>1106</v>
       </c>
       <c r="B42" s="10" t="s">
         <v>1111</v>
       </c>
       <c r="C42" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="F42" t="s">
         <v>122</v>
@@ -4774,13 +4783,13 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>1111</v>
       </c>
       <c r="C43" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="F43" t="s">
         <v>122</v>
@@ -4791,13 +4800,13 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>175</v>
+        <v>1115</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="C44" t="s">
-        <v>176</v>
+        <v>1116</v>
       </c>
       <c r="F44" t="s">
         <v>122</v>
@@ -4808,13 +4817,13 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B45" s="10" t="s">
         <v>1110</v>
       </c>
       <c r="C45" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F45" t="s">
         <v>122</v>
@@ -4825,145 +4834,145 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>161</v>
+        <v>1110</v>
       </c>
       <c r="C46" t="s">
-        <v>165</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="F46" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="G46" t="b">
         <v>0</v>
       </c>
-      <c r="H46">
-        <v>-60</v>
-      </c>
-      <c r="I46">
-        <v>30</v>
-      </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>1081</v>
+        <v>164</v>
       </c>
       <c r="B47" s="10" t="s">
         <v>161</v>
       </c>
       <c r="C47" t="s">
-        <v>163</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>160</v>
+        <v>165</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>186</v>
       </c>
       <c r="F47" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="G47" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>-60</v>
+      </c>
+      <c r="I47">
+        <v>30</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>161</v>
+        <v>1081</v>
       </c>
       <c r="B48" s="10" t="s">
         <v>161</v>
       </c>
       <c r="C48" t="s">
-        <v>162</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>186</v>
+        <v>163</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>160</v>
       </c>
       <c r="F48" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="G48" t="b">
-        <v>0</v>
-      </c>
-      <c r="H48">
-        <v>-90</v>
-      </c>
-      <c r="I48">
-        <v>60</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>1080</v>
+        <v>161</v>
       </c>
       <c r="B49" s="10" t="s">
         <v>161</v>
       </c>
       <c r="C49" t="s">
+        <v>162</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="F49" t="s">
+        <v>131</v>
+      </c>
+      <c r="G49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>-90</v>
+      </c>
+      <c r="I49">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="C50" t="s">
         <v>159</v>
       </c>
-      <c r="E49" s="10" t="s">
+      <c r="E50" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F50" t="s">
         <v>122</v>
       </c>
-      <c r="G49" t="b">
+      <c r="G50" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
+    <row r="51" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="s">
         <v>148</v>
-      </c>
-      <c r="B50" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="D50" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="F50" s="10" t="s">
-        <v>1056</v>
-      </c>
-      <c r="G50" s="10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>150</v>
       </c>
       <c r="B51" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="C51" t="s">
-        <v>151</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="F51" t="s">
-        <v>122</v>
-      </c>
-      <c r="G51" t="b">
+      <c r="C51" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G51" s="10" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B52" s="10" t="s">
         <v>141</v>
       </c>
       <c r="C52" t="s">
-        <v>147</v>
+        <v>151</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>183</v>
       </c>
       <c r="F52" t="s">
         <v>122</v>
@@ -4974,131 +4983,122 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="B53" s="10" t="s">
         <v>141</v>
       </c>
       <c r="C53" t="s">
-        <v>142</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
       <c r="F53" t="s">
-        <v>1056</v>
+        <v>122</v>
       </c>
       <c r="G53" t="b">
         <v>0</v>
       </c>
-      <c r="H53">
-        <v>0</v>
-      </c>
-      <c r="I53">
-        <v>99999</v>
-      </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="10" t="s">
-        <v>143</v>
+      <c r="A54" t="s">
+        <v>141</v>
       </c>
       <c r="B54" s="10" t="s">
         <v>141</v>
       </c>
       <c r="C54" t="s">
-        <v>144</v>
-      </c>
-      <c r="E54" s="10" t="s">
-        <v>145</v>
+        <v>142</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>184</v>
       </c>
       <c r="F54" t="s">
-        <v>122</v>
+        <v>1056</v>
       </c>
       <c r="G54" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>99999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="B55" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="C55" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="D55" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="F55" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="G55" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H55" s="10">
-        <v>0</v>
-      </c>
-      <c r="I55" s="10">
-        <v>99999</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>1068</v>
+      <c r="C55" t="s">
+        <v>144</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="F55" t="s">
+        <v>122</v>
+      </c>
+      <c r="G55" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
+        <v>155</v>
       </c>
       <c r="B56" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="C56" t="s">
-        <v>1069</v>
-      </c>
-      <c r="E56" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="F56" t="s">
-        <v>122</v>
+      <c r="C56" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>131</v>
       </c>
       <c r="G56" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="H56" s="10">
+        <v>0</v>
+      </c>
+      <c r="I56" s="10">
+        <v>99999</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>114</v>
+        <v>1068</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>1108</v>
+        <v>141</v>
       </c>
       <c r="C57" t="s">
-        <v>1070</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="F57" s="10" t="s">
-        <v>1056</v>
+        <v>1069</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="F57" t="s">
+        <v>122</v>
       </c>
       <c r="G57" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H57">
         <v>1</v>
-      </c>
-      <c r="I57">
-        <v>360</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B58" s="10" t="s">
         <v>1108</v>
       </c>
       <c r="C58" t="s">
-        <v>139</v>
+        <v>1070</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>183</v>
@@ -5118,13 +5118,13 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B59" s="10" t="s">
         <v>1108</v>
       </c>
       <c r="C59" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>183</v>
@@ -5144,16 +5144,16 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="B60" s="10" t="s">
         <v>1108</v>
       </c>
       <c r="C60" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>1067</v>
+        <v>183</v>
       </c>
       <c r="F60" s="10" t="s">
         <v>1056</v>
@@ -5162,81 +5162,107 @@
         <v>0</v>
       </c>
       <c r="H60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I60">
-        <v>100</v>
+        <v>360</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B61" s="10" t="s">
         <v>1108</v>
       </c>
-      <c r="C61" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="E61" s="10" t="s">
-        <v>138</v>
+      <c r="C61" t="s">
+        <v>133</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>1067</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>122</v>
+        <v>1056</v>
       </c>
       <c r="G61" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>100</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B62" s="10" t="s">
         <v>1108</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="G62" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>134</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C63" t="s">
         <v>135</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="D63" s="4" t="s">
         <v>1067</v>
       </c>
-      <c r="F62" s="10" t="s">
+      <c r="F63" s="10" t="s">
         <v>1056</v>
-      </c>
-      <c r="G62" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H62">
-        <v>0</v>
-      </c>
-      <c r="I62">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="B63" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="C63" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="D63" s="10"/>
-      <c r="F63" s="10" t="s">
-        <v>122</v>
       </c>
       <c r="G63" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="H63" s="10"/>
-      <c r="I63" s="10"/>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="D64" s="10"/>
+      <c r="F64" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="G64" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H64" s="10"/>
+      <c r="I64" s="10"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I63">
-    <sortCondition ref="B1:B63"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I64">
+    <sortCondition ref="B1:B64"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>